<commit_message>
Finished DBQ by Region Excel File
</commit_message>
<xml_diff>
--- a/Planning Documents/State_Pop_and_Vet_Pop_2016.xlsx
+++ b/Planning Documents/State_Pop_and_Vet_Pop_2016.xlsx
@@ -236,12 +236,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -557,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -568,9 +569,10 @@
     <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +586,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -599,7 +601,7 @@
         <v>6.6195457505279762</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -610,11 +612,11 @@
         <v>59121</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D51" si="0">(C3/B3)*100</f>
+        <f>(C3/B3)*100</f>
         <v>7.972925954995266</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -625,11 +627,11 @@
         <v>455815</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" si="0"/>
+        <f>(C4/B4)*100</f>
         <v>6.5977510486141853</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -640,11 +642,11 @@
         <v>196865</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="0"/>
+        <f>(C5/B5)*100</f>
         <v>6.5880114355282444</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -655,11 +657,11 @@
         <v>1591709</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="0"/>
+        <f>(C6/B6)*100</f>
         <v>4.0505133335620229</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -670,11 +672,11 @@
         <v>344469</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="0"/>
+        <f>(C7/B7)*100</f>
         <v>6.2289775691419962</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -685,11 +687,12 @@
         <v>177605</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="0"/>
+        <f>(C8/B8)*100</f>
         <v>4.9504067386072075</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -700,11 +703,11 @@
         <v>62879</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="0"/>
+        <f>(C9/B9)*100</f>
         <v>6.6000978274332471</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -715,11 +718,11 @@
         <v>1358575</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="0"/>
+        <f>(C10/B10)*100</f>
         <v>6.5769571152333031</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -730,11 +733,11 @@
         <v>588812</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="0"/>
+        <f>(C11/B11)*100</f>
         <v>5.7090720813836464</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -745,11 +748,11 @@
         <v>97496</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="0"/>
+        <f>(C12/B12)*100</f>
         <v>6.8241870309928805</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -760,11 +763,11 @@
         <v>110061</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="0"/>
+        <f>(C13/B13)*100</f>
         <v>6.5511486131762249</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -775,11 +778,11 @@
         <v>601286</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="0"/>
+        <f>(C14/B14)*100</f>
         <v>4.6844720742714516</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -790,11 +793,11 @@
         <v>384097</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="0"/>
+        <f>(C15/B15)*100</f>
         <v>5.7898190339564</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -805,7 +808,7 @@
         <v>190215</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="0"/>
+        <f>(C16/B16)*100</f>
         <v>6.0754697817123615</v>
       </c>
     </row>
@@ -820,7 +823,7 @@
         <v>178130</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="0"/>
+        <f>(C17/B17)*100</f>
         <v>6.1260825021296679</v>
       </c>
     </row>
@@ -835,7 +838,7 @@
         <v>268815</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="0"/>
+        <f>(C18/B18)*100</f>
         <v>6.0596968562342752</v>
       </c>
     </row>
@@ -850,7 +853,7 @@
         <v>245353</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="0"/>
+        <f>(C19/B19)*100</f>
         <v>5.2356973955418056</v>
       </c>
     </row>
@@ -865,7 +868,7 @@
         <v>106318</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="0"/>
+        <f>(C20/B20)*100</f>
         <v>7.9924404164085665</v>
       </c>
     </row>
@@ -880,7 +883,7 @@
         <v>346902</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="0"/>
+        <f>(C21/B21)*100</f>
         <v>5.757946551160944</v>
       </c>
     </row>
@@ -895,7 +898,7 @@
         <v>321371</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="0"/>
+        <f>(C22/B22)*100</f>
         <v>4.7096151791669092</v>
       </c>
     </row>
@@ -910,7 +913,7 @@
         <v>564615</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="0"/>
+        <f>(C23/B23)*100</f>
         <v>5.6839797270735373</v>
       </c>
     </row>
@@ -925,7 +928,7 @@
         <v>311234</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="0"/>
+        <f>(C24/B24)*100</f>
         <v>5.6331435914607102</v>
       </c>
     </row>
@@ -940,7 +943,7 @@
         <v>164336</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="0"/>
+        <f>(C25/B25)*100</f>
         <v>5.5046283347541296</v>
       </c>
     </row>
@@ -955,7 +958,7 @@
         <v>407329</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="0"/>
+        <f>(C26/B26)*100</f>
         <v>6.6871980057709708</v>
       </c>
     </row>
@@ -970,7 +973,7 @@
         <v>80615</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="0"/>
+        <f>(C27/B27)*100</f>
         <v>7.7614725183313817</v>
       </c>
     </row>
@@ -985,7 +988,7 @@
         <v>117241</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="0"/>
+        <f>(C28/B28)*100</f>
         <v>6.1459853019732096</v>
       </c>
     </row>
@@ -1000,7 +1003,7 @@
         <v>197580</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="0"/>
+        <f>(C29/B29)*100</f>
         <v>6.7221138424920071</v>
       </c>
     </row>
@@ -1015,7 +1018,7 @@
         <v>95826</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" si="0"/>
+        <f>(C30/B30)*100</f>
         <v>7.1778968775631737</v>
       </c>
     </row>
@@ -1030,7 +1033,7 @@
         <v>349335</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="0"/>
+        <f>(C31/B31)*100</f>
         <v>3.8908310775531008</v>
       </c>
     </row>
@@ -1045,7 +1048,7 @@
         <v>143962</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="0"/>
+        <f>(C32/B32)*100</f>
         <v>6.9032219703159825</v>
       </c>
     </row>
@@ -1060,7 +1063,7 @@
         <v>739116</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="0"/>
+        <f>(C33/B33)*100</f>
         <v>3.7260805777855794</v>
       </c>
     </row>
@@ -1075,7 +1078,7 @@
         <v>618330</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="0"/>
+        <f>(C34/B34)*100</f>
         <v>6.087909160160363</v>
       </c>
     </row>
@@ -1090,7 +1093,7 @@
         <v>45627</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="0"/>
+        <f>(C35/B35)*100</f>
         <v>6.0389280363391871</v>
       </c>
     </row>
@@ -1105,7 +1108,7 @@
         <v>725627</v>
       </c>
       <c r="D36" s="4">
-        <f t="shared" si="0"/>
+        <f>(C36/B36)*100</f>
         <v>6.2432663251123639</v>
       </c>
     </row>
@@ -1120,7 +1123,7 @@
         <v>263517</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" si="0"/>
+        <f>(C37/B37)*100</f>
         <v>6.720303212760764</v>
       </c>
     </row>
@@ -1135,7 +1138,7 @@
         <v>277996</v>
       </c>
       <c r="D38" s="4">
-        <f t="shared" si="0"/>
+        <f>(C38/B38)*100</f>
         <v>6.8036404405396098</v>
       </c>
     </row>
@@ -1150,7 +1153,7 @@
         <v>788496</v>
       </c>
       <c r="D39" s="4">
-        <f t="shared" si="0"/>
+        <f>(C39/B39)*100</f>
         <v>6.1663467475190785</v>
       </c>
     </row>
@@ -1165,7 +1168,7 @@
         <v>58949</v>
       </c>
       <c r="D40" s="4">
-        <f t="shared" si="0"/>
+        <f>(C40/B40)*100</f>
         <v>5.5740256400073376</v>
       </c>
     </row>
@@ -1180,7 +1183,7 @@
         <v>339776</v>
       </c>
       <c r="D41" s="4">
-        <f t="shared" si="0"/>
+        <f>(C41/B41)*100</f>
         <v>6.8505684276572829</v>
       </c>
     </row>
@@ -1195,7 +1198,7 @@
         <v>57227</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" si="0"/>
+        <f>(C42/B42)*100</f>
         <v>6.6423923616028002</v>
       </c>
     </row>
@@ -1210,7 +1213,7 @@
         <v>413852</v>
       </c>
       <c r="D43" s="4">
-        <f t="shared" si="0"/>
+        <f>(C43/B43)*100</f>
         <v>6.2238961567081796</v>
       </c>
     </row>
@@ -1225,7 +1228,7 @@
         <v>1364615</v>
       </c>
       <c r="D44" s="4">
-        <f t="shared" si="0"/>
+        <f>(C44/B44)*100</f>
         <v>4.8902409909785618</v>
       </c>
     </row>
@@ -1240,7 +1243,7 @@
         <v>121411</v>
       </c>
       <c r="D45" s="4">
-        <f t="shared" si="0"/>
+        <f>(C45/B45)*100</f>
         <v>3.9881142625892605</v>
       </c>
     </row>
@@ -1255,7 +1258,7 @@
         <v>39290</v>
       </c>
       <c r="D46" s="4">
-        <f t="shared" si="0"/>
+        <f>(C46/B46)*100</f>
         <v>6.3029995796930791</v>
       </c>
     </row>
@@ -1270,7 +1273,7 @@
         <v>607118</v>
       </c>
       <c r="D47" s="4">
-        <f t="shared" si="0"/>
+        <f>(C47/B47)*100</f>
         <v>7.2152434285116671</v>
       </c>
     </row>
@@ -1285,7 +1288,7 @@
         <v>501720</v>
       </c>
       <c r="D48" s="4">
-        <f t="shared" si="0"/>
+        <f>(C48/B48)*100</f>
         <v>6.8908741653199987</v>
       </c>
     </row>
@@ -1300,7 +1303,7 @@
         <v>136950</v>
       </c>
       <c r="D49" s="4">
-        <f t="shared" si="0"/>
+        <f>(C49/B49)*100</f>
         <v>7.4891845675221491</v>
       </c>
     </row>
@@ -1315,7 +1318,7 @@
         <v>341594</v>
       </c>
       <c r="D50" s="4">
-        <f t="shared" si="0"/>
+        <f>(C50/B50)*100</f>
         <v>5.9171819030136756</v>
       </c>
     </row>
@@ -1330,7 +1333,7 @@
         <v>43482</v>
       </c>
       <c r="D51" s="4">
-        <f t="shared" si="0"/>
+        <f>(C51/B51)*100</f>
         <v>7.4339641996204548</v>
       </c>
     </row>

</xml_diff>